<commit_message>
add site,add random read config,add some time print
</commit_message>
<xml_diff>
--- a/team/chunk/offer/cam4/config/c4mconfig.xlsx
+++ b/team/chunk/offer/cam4/config/c4mconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="8265"/>
+    <workbookView windowWidth="13140" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9">
   <si>
     <t>name</t>
   </si>
@@ -39,6 +39,9 @@
     <t>status</t>
   </si>
   <si>
+    <t>city</t>
+  </si>
+  <si>
     <t>site</t>
   </si>
 </sst>
@@ -47,10 +50,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -63,65 +66,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,6 +94,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,19 +172,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -214,6 +217,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -232,6 +265,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -281,84 +362,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,21 +408,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -443,26 +431,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,6 +467,41 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -513,10 +516,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -525,133 +528,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1007,19 +1010,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="4" max="4" width="10.375" customWidth="1"/>
     <col min="5" max="5" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1043,6 +1046,9 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
something is wrong with the github system
</commit_message>
<xml_diff>
--- a/team/chunk/offer/cam4/config/c4mconfig.xlsx
+++ b/team/chunk/offer/cam4/config/c4mconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13140" windowHeight="8805"/>
+    <workbookView windowWidth="20175" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
   <si>
     <t>name</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>site</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>asd@aol.com</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>http://www.baidu.com</t>
+  </si>
+  <si>
+    <t>asd@gmail.com</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>asd@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -64,6 +85,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -164,14 +193,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -186,23 +207,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,6 +238,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -235,72 +412,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -308,96 +419,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,10 +537,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -528,138 +549,141 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1010,13 +1034,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
     <col min="4" max="4" width="10.375" customWidth="1"/>
     <col min="5" max="5" width="13.75" customWidth="1"/>
@@ -1051,7 +1075,67 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="2:9">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="asd@aol.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="asd@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="asd@yahoo.com"/>
+    <hyperlink ref="I2" r:id="rId4" display="http://www.baidu.com"/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>